<commit_message>
Arduino Code + Sensor Code - Have to tune PID - Use motorLibv5
</commit_message>
<xml_diff>
--- a/Arduino/Motor Stats.xlsx
+++ b/Arduino/Motor Stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonah\Documents\MDP18Forever\Arduino\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C1669AF-B710-4C28-87AB-EA8299462F8A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{713A5F02-A001-45BD-A6F9-23643D5285C8}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="2688" firstSheet="1" activeTab="2" xr2:uid="{A5756DC7-64DE-4789-A5A0-903E8564F046}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="2688" firstSheet="1" activeTab="1" xr2:uid="{A5756DC7-64DE-4789-A5A0-903E8564F046}"/>
   </bookViews>
   <sheets>
     <sheet name="Cycle Measurement" sheetId="2" r:id="rId1"/>
@@ -178,15 +178,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -195,6 +186,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2725,8 +2725,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="6"/>
-      <c r="B1" s="7"/>
+      <c r="A1" s="12"/>
+      <c r="B1" s="13"/>
       <c r="C1" s="1" t="s">
         <v>7</v>
       </c>
@@ -2735,7 +2735,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="11" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -2749,7 +2749,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="5"/>
+      <c r="A3" s="11"/>
       <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
@@ -2761,7 +2761,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="11" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -2777,7 +2777,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="5"/>
+      <c r="A5" s="11"/>
       <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
@@ -2791,7 +2791,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="11" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -2807,7 +2807,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="5"/>
+      <c r="A7" s="11"/>
       <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
@@ -2821,7 +2821,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="11" t="s">
         <v>1</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -2837,7 +2837,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="5"/>
+      <c r="A9" s="11"/>
       <c r="B9" s="1" t="s">
         <v>5</v>
       </c>
@@ -2883,7 +2883,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A538ED70-E746-44A9-82E1-59856942DFFF}">
   <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -2893,33 +2893,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5" t="s">
+      <c r="A2" s="11"/>
+      <c r="B2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5" t="s">
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" s="5"/>
+      <c r="A3" s="11"/>
       <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
@@ -2938,12 +2938,12 @@
       <c r="G3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="9" t="s">
+      <c r="H3" s="6" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" s="8">
+      <c r="A4" s="5">
         <v>0</v>
       </c>
       <c r="B4" s="1">
@@ -2966,7 +2966,7 @@
         <f>(E4+F4)/2</f>
         <v>0</v>
       </c>
-      <c r="H4" s="10">
+      <c r="H4" s="7">
         <f>D4-G4</f>
         <v>0</v>
       </c>
@@ -2995,7 +2995,7 @@
         <f>(E5+F5)/2</f>
         <v>15.05</v>
       </c>
-      <c r="H5" s="10">
+      <c r="H5" s="7">
         <f t="shared" ref="H5:H12" si="0">D5-G5</f>
         <v>1.1449999999999996</v>
       </c>
@@ -3025,7 +3025,7 @@
         <f t="shared" ref="G6:G12" si="2">(E6+F6)/2</f>
         <v>32.69</v>
       </c>
-      <c r="H6" s="10">
+      <c r="H6" s="7">
         <f t="shared" si="0"/>
         <v>1.4849999999999994</v>
       </c>
@@ -3062,7 +3062,7 @@
         <f t="shared" si="2"/>
         <v>52.045000000000002</v>
       </c>
-      <c r="H7" s="10">
+      <c r="H7" s="7">
         <f t="shared" si="0"/>
         <v>1.1049999999999969</v>
       </c>
@@ -3092,7 +3092,7 @@
         <f t="shared" si="2"/>
         <v>71.474999999999994</v>
       </c>
-      <c r="H8" s="10">
+      <c r="H8" s="7">
         <f t="shared" si="0"/>
         <v>1.2900000000000063</v>
       </c>
@@ -3122,7 +3122,7 @@
         <f t="shared" si="2"/>
         <v>92.05</v>
       </c>
-      <c r="H9" s="10">
+      <c r="H9" s="7">
         <f t="shared" si="0"/>
         <v>1.0700000000000074</v>
       </c>
@@ -3152,7 +3152,7 @@
         <f t="shared" si="2"/>
         <v>113.12</v>
       </c>
-      <c r="H10" s="10">
+      <c r="H10" s="7">
         <f t="shared" si="0"/>
         <v>0.72499999999999432</v>
       </c>
@@ -3182,7 +3182,7 @@
         <f t="shared" si="2"/>
         <v>132.61500000000001</v>
       </c>
-      <c r="H11" s="10">
+      <c r="H11" s="7">
         <f t="shared" si="0"/>
         <v>2.9999999999972715E-2</v>
       </c>
@@ -3212,128 +3212,128 @@
         <f t="shared" si="2"/>
         <v>143.84500000000003</v>
       </c>
-      <c r="H12" s="10">
+      <c r="H12" s="7">
         <f t="shared" si="0"/>
         <v>-1.2800000000000296</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="11"/>
+      <c r="A17" s="8"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="11" t="s">
+      <c r="A18" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B18" s="12" t="s">
+      <c r="B18" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="12" t="s">
+      <c r="C18" s="9" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="13">
+      <c r="A19" s="10">
         <v>0</v>
       </c>
-      <c r="B19" s="12">
+      <c r="B19" s="9">
         <v>0</v>
       </c>
-      <c r="C19" s="12">
+      <c r="C19" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="12">
+      <c r="A20" s="9">
         <v>50</v>
       </c>
-      <c r="B20" s="12">
+      <c r="B20" s="9">
         <v>16.195</v>
       </c>
-      <c r="C20" s="12">
+      <c r="C20" s="9">
         <v>15.05</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="12">
+      <c r="A21" s="9">
         <f>A20+50</f>
         <v>100</v>
       </c>
-      <c r="B21" s="12">
+      <c r="B21" s="9">
         <v>34.174999999999997</v>
       </c>
-      <c r="C21" s="12">
+      <c r="C21" s="9">
         <v>32.69</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="12">
+      <c r="A22" s="9">
         <f t="shared" ref="A22:A26" si="4">A21+50</f>
         <v>150</v>
       </c>
-      <c r="B22" s="12">
+      <c r="B22" s="9">
         <v>53.15</v>
       </c>
-      <c r="C22" s="12">
+      <c r="C22" s="9">
         <v>52.045000000000002</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="12">
+      <c r="A23" s="9">
         <f t="shared" si="4"/>
         <v>200</v>
       </c>
-      <c r="B23" s="12">
+      <c r="B23" s="9">
         <v>72.765000000000001</v>
       </c>
-      <c r="C23" s="12">
+      <c r="C23" s="9">
         <v>71.474999999999994</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="12">
+      <c r="A24" s="9">
         <f t="shared" si="4"/>
         <v>250</v>
       </c>
-      <c r="B24" s="12">
+      <c r="B24" s="9">
         <v>93.12</v>
       </c>
-      <c r="C24" s="12">
+      <c r="C24" s="9">
         <v>92.05</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="12">
+      <c r="A25" s="9">
         <f t="shared" si="4"/>
         <v>300</v>
       </c>
-      <c r="B25" s="12">
+      <c r="B25" s="9">
         <v>113.845</v>
       </c>
-      <c r="C25" s="12">
+      <c r="C25" s="9">
         <v>113.12</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="12">
+      <c r="A26" s="9">
         <f t="shared" si="4"/>
         <v>350</v>
       </c>
-      <c r="B26" s="12">
+      <c r="B26" s="9">
         <v>132.64499999999998</v>
       </c>
-      <c r="C26" s="12">
+      <c r="C26" s="9">
         <v>132.61500000000001</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" s="12">
+      <c r="A27" s="9">
         <f>A26+50</f>
         <v>400</v>
       </c>
-      <c r="B27" s="12">
+      <c r="B27" s="9">
         <v>142.565</v>
       </c>
-      <c r="C27" s="12">
+      <c r="C27" s="9">
         <v>143.84500000000003</v>
       </c>
     </row>
@@ -3353,7 +3353,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{209CC328-9633-43B9-9A37-AD00E7B67D8C}">
   <dimension ref="A1:A154"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A122" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A122" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="B130" sqref="B130"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
MotorLibv7 - Quite accurate
</commit_message>
<xml_diff>
--- a/Arduino/Motor Stats.xlsx
+++ b/Arduino/Motor Stats.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonah\Documents\MDP18Forever\Arduino\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{713A5F02-A001-45BD-A6F9-23643D5285C8}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36D92EE2-1F44-441C-85C1-A1E8DB6AE888}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="2688" firstSheet="1" activeTab="1" xr2:uid="{A5756DC7-64DE-4789-A5A0-903E8564F046}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17250" windowHeight="2685" firstSheet="1" activeTab="1" xr2:uid="{A5756DC7-64DE-4789-A5A0-903E8564F046}"/>
   </bookViews>
   <sheets>
     <sheet name="Cycle Measurement" sheetId="2" r:id="rId1"/>
@@ -2718,13 +2718,13 @@
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="12"/>
       <c r="B1" s="13"/>
       <c r="C1" s="1" t="s">
@@ -2734,7 +2734,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>9</v>
       </c>
@@ -2748,7 +2748,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="11"/>
       <c r="B3" s="1" t="s">
         <v>5</v>
@@ -2760,7 +2760,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>10</v>
       </c>
@@ -2776,7 +2776,7 @@
         <v>882</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="11"/>
       <c r="B5" s="1" t="s">
         <v>5</v>
@@ -2790,7 +2790,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>13</v>
       </c>
@@ -2806,7 +2806,7 @@
         <v>0.49590450000000003</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="11"/>
       <c r="B7" s="1" t="s">
         <v>5</v>
@@ -2820,7 +2820,7 @@
         <v>0.55550299999999997</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>1</v>
       </c>
@@ -2836,7 +2836,7 @@
         <v>120.99103758889061</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="11"/>
       <c r="B9" s="1" t="s">
         <v>5</v>
@@ -2850,7 +2850,7 @@
         <v>108.01021776660073</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
@@ -2858,7 +2858,7 @@
         <v>562.25</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
@@ -2881,18 +2881,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A538ED70-E746-44A9-82E1-59856942DFFF}">
-  <dimension ref="A1:L27"/>
+  <dimension ref="A1:M27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -2905,7 +2905,7 @@
       <c r="F1" s="11"/>
       <c r="G1" s="11"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="11"/>
       <c r="B2" s="11" t="s">
         <v>2</v>
@@ -2918,7 +2918,7 @@
       <c r="F2" s="11"/>
       <c r="G2" s="11"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="11"/>
       <c r="B3" s="1" t="s">
         <v>6</v>
@@ -2942,7 +2942,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>0</v>
       </c>
@@ -2971,7 +2971,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>50</v>
       </c>
@@ -2999,8 +2999,20 @@
         <f t="shared" ref="H5:H12" si="0">D5-G5</f>
         <v>1.1449999999999996</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="I5">
+        <f>D5/A5</f>
+        <v>0.32390000000000002</v>
+      </c>
+      <c r="J5">
+        <f>G5/A5</f>
+        <v>0.30099999999999999</v>
+      </c>
+      <c r="K5">
+        <f>AVERAGE(I5:J5)</f>
+        <v>0.31245000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <f>A5+50</f>
         <v>100</v>
@@ -3029,17 +3041,29 @@
         <f t="shared" si="0"/>
         <v>1.4849999999999994</v>
       </c>
-      <c r="K6" t="s">
+      <c r="I6">
+        <f t="shared" ref="I6:I11" si="3">D6/A6</f>
+        <v>0.34175</v>
+      </c>
+      <c r="J6">
+        <f t="shared" ref="J6:J11" si="4">G6/A6</f>
+        <v>0.32689999999999997</v>
+      </c>
+      <c r="K6">
+        <f t="shared" ref="K6:K12" si="5">AVERAGE(I6:J6)</f>
+        <v>0.33432499999999998</v>
+      </c>
+      <c r="L6" t="s">
         <v>16</v>
       </c>
-      <c r="L6">
+      <c r="M6">
         <f>(D10-D9)/50</f>
         <v>0.41449999999999987</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <f t="shared" ref="A7:A11" si="3">A6+50</f>
+        <f t="shared" ref="A7:A11" si="6">A6+50</f>
         <v>150</v>
       </c>
       <c r="B7" s="2">
@@ -3066,10 +3090,22 @@
         <f t="shared" si="0"/>
         <v>1.1049999999999969</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="I7">
+        <f t="shared" si="3"/>
+        <v>0.35433333333333333</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="4"/>
+        <v>0.3469666666666667</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="5"/>
+        <v>0.35065000000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>200</v>
       </c>
       <c r="B8" s="2">
@@ -3096,10 +3132,22 @@
         <f t="shared" si="0"/>
         <v>1.2900000000000063</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="I8">
+        <f t="shared" si="3"/>
+        <v>0.36382500000000001</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="4"/>
+        <v>0.357375</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="5"/>
+        <v>0.36060000000000003</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>250</v>
       </c>
       <c r="B9" s="2">
@@ -3126,10 +3174,22 @@
         <f t="shared" si="0"/>
         <v>1.0700000000000074</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="I9">
+        <f t="shared" si="3"/>
+        <v>0.37248000000000003</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="4"/>
+        <v>0.36819999999999997</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="5"/>
+        <v>0.37034</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>300</v>
       </c>
       <c r="B10" s="2">
@@ -3156,10 +3216,22 @@
         <f t="shared" si="0"/>
         <v>0.72499999999999432</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="I10">
+        <f t="shared" si="3"/>
+        <v>0.37948333333333334</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="4"/>
+        <v>0.37706666666666666</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="5"/>
+        <v>0.37827500000000003</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>350</v>
       </c>
       <c r="B11" s="2">
@@ -3186,8 +3258,20 @@
         <f t="shared" si="0"/>
         <v>2.9999999999972715E-2</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="I11">
+        <f t="shared" si="3"/>
+        <v>0.37898571428571426</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="4"/>
+        <v>0.37890000000000001</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="5"/>
+        <v>0.37894285714285714</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <f>A11+50</f>
         <v>400</v>
@@ -3216,11 +3300,29 @@
         <f t="shared" si="0"/>
         <v>-1.2800000000000296</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="I12">
+        <f>D12/A12</f>
+        <v>0.35641250000000002</v>
+      </c>
+      <c r="J12">
+        <f>G12/A12</f>
+        <v>0.35961250000000006</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="5"/>
+        <v>0.35801250000000007</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K13">
+        <f>AVERAGE(K5:K12)</f>
+        <v>0.35544941964285715</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="8"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
         <v>0</v>
       </c>
@@ -3231,7 +3333,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="10">
         <v>0</v>
       </c>
@@ -3242,7 +3344,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="9">
         <v>50</v>
       </c>
@@ -3253,7 +3355,7 @@
         <v>15.05</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="9">
         <f>A20+50</f>
         <v>100</v>
@@ -3265,9 +3367,9 @@
         <v>32.69</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="9">
-        <f t="shared" ref="A22:A26" si="4">A21+50</f>
+        <f t="shared" ref="A22:A26" si="7">A21+50</f>
         <v>150</v>
       </c>
       <c r="B22" s="9">
@@ -3277,9 +3379,9 @@
         <v>52.045000000000002</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>200</v>
       </c>
       <c r="B23" s="9">
@@ -3289,9 +3391,9 @@
         <v>71.474999999999994</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>250</v>
       </c>
       <c r="B24" s="9">
@@ -3301,9 +3403,9 @@
         <v>92.05</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>300</v>
       </c>
       <c r="B25" s="9">
@@ -3313,9 +3415,9 @@
         <v>113.12</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>350</v>
       </c>
       <c r="B26" s="9">
@@ -3325,7 +3427,7 @@
         <v>132.61500000000001</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="9">
         <f>A26+50</f>
         <v>400</v>
@@ -3357,774 +3459,774 @@
       <selection activeCell="B130" sqref="B130"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>33.94</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>33.94</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>32.22</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>32.22</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>32.22</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>33.86</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>33.86</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>35.57</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>37.26</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>38.33</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>40.92</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>45.53</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>42.35</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>44.46</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>43.88</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>47.14</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>45.53</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>45.84</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>45.68</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>46.8</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>47.98</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>49.96</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>49.96</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>51.11</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>48.33</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>49.22</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>51.11</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>51.3</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>48.33</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>49.77</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>51.7</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>50.34</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>49.04</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>50.53</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>49.96</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>50.91</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>51.11</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>51.9</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>51.11</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>53.14</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>50.34</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>51.5</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>52.72</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>52.52</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>52.72</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>49.4</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>50.72</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>52.72</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>50.15</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>51.11</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51.5</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>53.57</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53.57</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>50.53</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>51.3</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>51.7</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>50.15</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>51.7</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>50.91</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>51.7</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>51.7</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>51.11</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>51.3</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>51.3</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>53.79</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>50.53</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>51.3</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>51.7</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>52.72</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>51.7</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>53.57</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>50.72</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>51.9</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>52.52</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>49.77</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>52.93</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>49.77</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>51.11</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>52.93</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>50.53</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>51.9</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>50.91</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>51.5</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>53.79</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>50.72</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>51.5</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>52.11</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>50.15</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>52.11</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>50.91</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>51.7</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>51.9</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>50.34</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>53.14</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>53.14</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>49.77</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>51.11</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>53.14</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>50.53</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>58.51</v>
       </c>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>51.7</v>
       </c>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>53.79</v>
       </c>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>50.91</v>
       </c>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>51.9</v>
       </c>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>52.52</v>
       </c>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>51.3</v>
       </c>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>50.15</v>
       </c>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>51.7</v>
       </c>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>50.91</v>
       </c>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>51.7</v>
       </c>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>51.9</v>
       </c>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>51.11</v>
       </c>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>50.91</v>
       </c>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>51.3</v>
       </c>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>53.79</v>
       </c>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>50.53</v>
       </c>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>51.5</v>
       </c>
     </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>51.7</v>
       </c>
     </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>51.9</v>
       </c>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>51.7</v>
       </c>
     </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>53.79</v>
       </c>
     </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>50.91</v>
       </c>
     </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>51.9</v>
       </c>
     </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>52.52</v>
       </c>
     </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>52.93</v>
       </c>
     </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>51.5</v>
       </c>
     </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>49.59</v>
       </c>
     </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>51.11</v>
       </c>
     </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>52.93</v>
       </c>
     </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>50.34</v>
       </c>
     </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>52.52</v>
       </c>
     </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>51.7</v>
       </c>
     </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>53.57</v>
       </c>
     </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>59.82</v>
       </c>
     </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>50.53</v>
       </c>
     </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>51.3</v>
       </c>
     </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>51.7</v>
       </c>
     </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>50.15</v>
       </c>
     </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>51.5</v>
       </c>
     </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>50.91</v>
       </c>
     </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>51.3</v>
       </c>
     </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>51.7</v>
       </c>
     </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>51.11</v>
       </c>
     </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>50.91</v>
       </c>
     </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>51.3</v>
       </c>
     </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>53.57</v>
       </c>
     </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>50.34</v>
       </c>
     </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>52.93</v>
       </c>
     </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>50.53</v>
       </c>
     </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>52.72</v>
       </c>
     </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>51.7</v>
       </c>
     </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>53.79</v>
       </c>
     </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>50.91</v>
       </c>

</xml_diff>